<commit_message>
Excel report generation order by asc
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/report.xlsx
+++ b/src/Controllers/Sheet/report.xlsx
@@ -139,10 +139,10 @@
     <t xml:space="preserve">CNY</t>
   </si>
   <si>
-    <t xml:space="preserve">01/11/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23:41</t>
+    <t xml:space="preserve">02/11/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:03</t>
   </si>
 </sst>
 </file>

</xml_diff>